<commit_message>
include fuel tax option improve average transport work values
</commit_message>
<xml_diff>
--- a/input_data/ship_eff+transportwork.xlsx
+++ b/input_data/ship_eff+transportwork.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="75">
   <si>
     <t>Average transport work per ship type</t>
   </si>
@@ -239,6 +239,12 @@
   </si>
   <si>
     <t>average over size</t>
+  </si>
+  <si>
+    <t>ton*NM</t>
+  </si>
+  <si>
+    <t>gigaton*NM</t>
   </si>
 </sst>
 </file>
@@ -327,14 +333,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>55034</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>370771</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>243771</xdr:colOff>
       <xdr:row>35</xdr:row>
       <xdr:rowOff>54677</xdr:rowOff>
     </xdr:to>
@@ -365,13 +371,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>22</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>43392</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>172508</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
+      <xdr:col>31</xdr:col>
       <xdr:colOff>580349</xdr:colOff>
       <xdr:row>44</xdr:row>
       <xdr:rowOff>57198</xdr:rowOff>
@@ -862,853 +868,959 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:AK115"/>
+  <dimension ref="A2:AL115"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="P41" sqref="P41"/>
+      <selection activeCell="F10" sqref="F10:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.28515625" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="I2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J2">
         <v>1</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3">
         <v>1.8520000000000001</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
         <v>53</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="J4" t="s">
+      <c r="I4" s="1"/>
+      <c r="K4" t="s">
         <v>63</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>3</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>4</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>5</v>
-      </c>
-      <c r="K5" t="s">
-        <v>67</v>
       </c>
       <c r="L5" t="s">
         <v>67</v>
       </c>
       <c r="M5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N5" t="s">
         <v>58</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>2012</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <v>2050</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B6" s="3">
-        <v>3</v>
-      </c>
-      <c r="C6" s="3">
-        <v>7</v>
-      </c>
-      <c r="D6" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="E6" s="3">
-        <v>4</v>
-      </c>
-      <c r="F6" s="3">
-        <v>0.3</v>
-      </c>
-      <c r="J6" s="1" t="s">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="K6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
       <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
         <v>999</v>
       </c>
-      <c r="M6" s="5">
+      <c r="N6" s="5">
         <v>179809363</v>
       </c>
-      <c r="N6" s="7">
+      <c r="O6" s="7">
         <v>0.22</v>
       </c>
-      <c r="O6">
-        <f>+M6*N6</f>
+      <c r="P6">
+        <f>+N6*O6</f>
         <v>39558059.859999999</v>
       </c>
-      <c r="P6" s="8">
+      <c r="Q6" s="8">
         <v>0.22</v>
       </c>
-      <c r="Q6">
-        <f>+M6*P6</f>
+      <c r="R6">
+        <f>+N6*Q6</f>
         <v>39558059.859999999</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B7" s="4">
-        <f>+B6*$I$3</f>
-        <v>5.556</v>
-      </c>
-      <c r="C7" s="4">
-        <f>+C6*$I$3</f>
-        <v>12.964</v>
-      </c>
-      <c r="D7" s="4">
-        <f t="shared" ref="C7:F7" si="0">+D6*$I$3</f>
-        <v>0.92600000000000005</v>
-      </c>
-      <c r="E7" s="4">
-        <f>+E6*$I$3</f>
-        <v>7.4080000000000004</v>
-      </c>
-      <c r="F7" s="4">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="L7">
+        <v>1000</v>
+      </c>
+      <c r="M7">
+        <v>1999</v>
+      </c>
+      <c r="N7" s="5">
+        <v>578339367</v>
+      </c>
+      <c r="O7" s="8">
+        <v>0.25</v>
+      </c>
+      <c r="P7">
+        <f>+N7*O7</f>
+        <v>144584841.75</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>0.2</v>
+      </c>
+      <c r="R7">
+        <f>+N7*Q7</f>
+        <v>115667873.40000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8">
+        <v>2012</v>
+      </c>
+      <c r="C8" s="5">
+        <f>+SUM(P26:P33)</f>
+        <v>8622401013.4399986</v>
+      </c>
+      <c r="D8" s="5">
+        <f>+SUM(P17:P22)</f>
+        <v>5207608850.96</v>
+      </c>
+      <c r="E8">
+        <v>365344150</v>
+      </c>
+      <c r="F8" s="5">
+        <f>+SUM(P6:P13)</f>
+        <v>2033999167.0540001</v>
+      </c>
+      <c r="G8">
+        <v>820375271</v>
+      </c>
+      <c r="L8">
+        <v>2000</v>
+      </c>
+      <c r="M8">
+        <v>2999</v>
+      </c>
+      <c r="N8" s="5">
+        <v>1480205694</v>
+      </c>
+      <c r="O8" s="8">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="P8">
+        <f t="shared" ref="P8:P9" si="0">+N8*O8</f>
+        <v>207228797.16000003</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>0.18</v>
+      </c>
+      <c r="R8">
+        <f t="shared" ref="R8:R13" si="1">+N8*Q8</f>
+        <v>266437024.91999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>73</v>
+      </c>
+      <c r="B9">
+        <v>2050</v>
+      </c>
+      <c r="C9" s="5">
+        <f>+SUM(R26:R33)</f>
+        <v>8622401013.4399986</v>
+      </c>
+      <c r="D9" s="5">
+        <f>+SUM(R17:R22)</f>
+        <v>5599732634.3800001</v>
+      </c>
+      <c r="E9">
+        <v>365344150</v>
+      </c>
+      <c r="F9" s="5">
+        <f>+SUM(R6:R13)</f>
+        <v>2700751170.7999997</v>
+      </c>
+      <c r="G9">
+        <v>820375271</v>
+      </c>
+      <c r="L9">
+        <v>3000</v>
+      </c>
+      <c r="M9">
+        <v>4999</v>
+      </c>
+      <c r="N9" s="5">
+        <v>2820323533</v>
+      </c>
+      <c r="O9" s="8">
+        <v>0.19</v>
+      </c>
+      <c r="P9">
         <f t="shared" si="0"/>
-        <v>0.55559999999999998</v>
-      </c>
-      <c r="K7">
-        <v>1000</v>
-      </c>
-      <c r="L7">
-        <v>1999</v>
-      </c>
-      <c r="M7" s="5">
-        <v>578339367</v>
-      </c>
-      <c r="N7" s="8">
-        <v>0.25</v>
-      </c>
-      <c r="O7">
-        <f t="shared" ref="O7:O9" si="1">+M7*N7</f>
-        <v>144584841.75</v>
-      </c>
-      <c r="P7" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" ref="Q7:Q20" si="2">+M7*P7</f>
-        <v>115667873.40000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A8">
+        <v>535861471.26999998</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>0.05</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="1"/>
+        <v>141016176.65000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>74</v>
+      </c>
+      <c r="B10">
         <v>2012</v>
-      </c>
-      <c r="B8" s="5">
-        <v>7000000000</v>
-      </c>
-      <c r="C8" s="5">
-        <f>+SUM(O17:O22)</f>
-        <v>5207608850.96</v>
-      </c>
-      <c r="E8" s="5">
-        <f>+SUM(O6:O13)</f>
-        <v>2033999167.0540001</v>
-      </c>
-      <c r="K8">
-        <v>2000</v>
-      </c>
-      <c r="L8">
-        <v>2999</v>
-      </c>
-      <c r="M8" s="5">
-        <v>1480205694</v>
-      </c>
-      <c r="N8" s="8">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="O8">
-        <f t="shared" si="1"/>
-        <v>207228797.16000003</v>
-      </c>
-      <c r="P8" s="8">
-        <v>0.18</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" si="2"/>
-        <v>266437024.91999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2050</v>
-      </c>
-      <c r="B9" s="5">
-        <v>7000000000</v>
-      </c>
-      <c r="C9" s="5">
-        <f>+SUM(Q17:Q22)</f>
-        <v>5599732634.3800001</v>
-      </c>
-      <c r="E9" s="5">
-        <f>+SUM(Q6:Q13)</f>
-        <v>2700751170.7999997</v>
-      </c>
-      <c r="K9">
-        <v>3000</v>
-      </c>
-      <c r="L9">
-        <v>4999</v>
-      </c>
-      <c r="M9" s="5">
-        <v>2820323533</v>
-      </c>
-      <c r="N9" s="8">
-        <v>0.19</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="1"/>
-        <v>535861471.26999998</v>
-      </c>
-      <c r="P9" s="8">
-        <v>0.05</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="2"/>
-        <v>141016176.65000001</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2012</v>
-      </c>
-      <c r="B10">
-        <f>+B8/1000000000</f>
-        <v>7</v>
       </c>
       <c r="C10" s="9">
         <f>+C8/1000000000</f>
+        <v>8.6224010134399993</v>
+      </c>
+      <c r="D10" s="9">
+        <f>+D8/1000000000</f>
         <v>5.2076088509599998</v>
       </c>
       <c r="E10" s="9">
         <f>+E8/1000000000</f>
+        <v>0.36534414999999998</v>
+      </c>
+      <c r="F10" s="9">
+        <f>+F8/1000000000</f>
         <v>2.0339991670540001</v>
       </c>
-      <c r="K10">
+      <c r="G10" s="9">
+        <f>+G8/1000000000</f>
+        <v>0.82037527099999996</v>
+      </c>
+      <c r="L10">
         <v>5000</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>7999</v>
       </c>
-      <c r="M10" s="5">
+      <c r="N10" s="5">
         <v>4233489679</v>
       </c>
-      <c r="N10" s="8">
+      <c r="O10" s="8">
         <v>0.11</v>
       </c>
-      <c r="O10">
-        <f>+M10*N10</f>
+      <c r="P10">
+        <f>+N10*O10</f>
         <v>465683864.69</v>
       </c>
-      <c r="P10" s="8">
+      <c r="Q10" s="8">
         <v>0.11</v>
       </c>
-      <c r="Q10">
-        <f t="shared" si="2"/>
+      <c r="R10">
+        <f t="shared" si="1"/>
         <v>465683864.69</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>74</v>
+      </c>
+      <c r="B11">
         <v>2050</v>
-      </c>
-      <c r="B11">
-        <f>+B9/1000000000</f>
-        <v>7</v>
       </c>
       <c r="C11" s="9">
         <f>+C9/1000000000</f>
+        <v>8.6224010134399993</v>
+      </c>
+      <c r="D11" s="9">
+        <f>+D9/1000000000</f>
         <v>5.5997326343800005</v>
       </c>
       <c r="E11" s="9">
         <f>+E9/1000000000</f>
+        <v>0.36534414999999998</v>
+      </c>
+      <c r="F11" s="9">
+        <f>+F9/1000000000</f>
         <v>2.7007511707999998</v>
       </c>
-      <c r="K11">
+      <c r="G11" s="9">
+        <f>+G9/1000000000</f>
+        <v>0.82037527099999996</v>
+      </c>
+      <c r="L11">
         <v>8000</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>11999</v>
       </c>
-      <c r="M11" s="5">
+      <c r="N11" s="5">
         <v>6968284047</v>
       </c>
-      <c r="N11" s="8">
+      <c r="O11" s="8">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="O11">
-        <f>+M11*N11</f>
+      <c r="P11">
+        <f>+N11*O11</f>
         <v>487779883.29000002</v>
       </c>
-      <c r="P11" s="8">
+      <c r="Q11" s="8">
         <v>0.1</v>
       </c>
-      <c r="Q11">
-        <f t="shared" si="2"/>
+      <c r="R11">
+        <f t="shared" si="1"/>
         <v>696828404.70000005</v>
       </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K12">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="L12">
         <v>12000</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>14500</v>
       </c>
-      <c r="M12" s="5">
+      <c r="N12" s="5">
         <v>6968284047</v>
       </c>
-      <c r="N12" s="8">
+      <c r="O12" s="8">
         <v>0.02</v>
       </c>
-      <c r="O12">
-        <f t="shared" ref="O12" si="3">+M12*N12</f>
+      <c r="P12">
+        <f t="shared" ref="P12" si="2">+N12*O12</f>
         <v>139365680.94</v>
       </c>
-      <c r="P12" s="8">
+      <c r="Q12" s="8">
         <v>0.09</v>
       </c>
-      <c r="Q12">
-        <f t="shared" si="2"/>
+      <c r="R12">
+        <f t="shared" si="1"/>
         <v>627145564.23000002</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K13">
-        <v>14500</v>
-      </c>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L13">
         <v>14500</v>
       </c>
-      <c r="M13" s="5">
+      <c r="M13">
+        <v>14500</v>
+      </c>
+      <c r="N13" s="5">
         <v>6968284047</v>
       </c>
-      <c r="N13" s="8">
+      <c r="O13" s="8">
         <v>2E-3</v>
       </c>
-      <c r="O13" s="10">
-        <f>+M13*N13</f>
+      <c r="P13" s="10">
+        <f>+N13*O13</f>
         <v>13936568.094000001</v>
       </c>
-      <c r="P13" s="8">
+      <c r="Q13" s="8">
         <v>0.05</v>
       </c>
-      <c r="Q13">
-        <f t="shared" si="2"/>
+      <c r="R13">
+        <f t="shared" si="1"/>
         <v>348414202.35000002</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J14" t="s">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="K14" t="s">
         <v>71</v>
       </c>
-      <c r="M14" s="5"/>
-      <c r="N14" s="10">
-        <f>+AVERAGE(K6:L6)*N6+AVERAGE(K7:L7)*N7+AVERAGE(K8:L8)*N8+AVERAGE(K9:L9)*N9+AVERAGE(K10:L10)*N10+AVERAGE(K11:L11)*N11+AVERAGE(K12:L12)*N12+AVERAGE(K13:L13)*N13</f>
+      <c r="N14" s="5"/>
+      <c r="O14" s="10">
+        <f>+AVERAGE(L6:M6)*O6+AVERAGE(L7:M7)*O7+AVERAGE(L8:M8)*O8+AVERAGE(L9:M9)*O9+AVERAGE(L10:M10)*O10+AVERAGE(L11:M11)*O11+AVERAGE(L12:M12)*O12+AVERAGE(L13:M13)*O13</f>
         <v>3303.51</v>
       </c>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10">
-        <f>+AVERAGE(K6:L6)*P6+AVERAGE(K7:L7)*P7+AVERAGE(K8:L8)*P8+AVERAGE(K9:L9)*P9+AVERAGE(K10:L10)*P10+AVERAGE(K11:L11)*P11+AVERAGE(K12:L12)*P12+AVERAGE(K13:L13)*P13</f>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10">
+        <f>+AVERAGE(L6:M6)*Q6+AVERAGE(L7:M7)*Q7+AVERAGE(L8:M8)*Q8+AVERAGE(L9:M9)*Q9+AVERAGE(L10:M10)*Q10+AVERAGE(L11:M11)*Q11+AVERAGE(L12:M12)*Q12+AVERAGE(L13:M13)*Q13</f>
         <v>4692.0700000000006</v>
       </c>
-      <c r="R14" s="10">
-        <f>+AVERAGE(N14:P14)</f>
+      <c r="S14" s="10">
+        <f>+AVERAGE(O14:Q14)</f>
         <v>3997.7900000000004</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="M15" s="5"/>
-      <c r="N15" s="10"/>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="N15" s="5"/>
       <c r="O15" s="10"/>
       <c r="P15" s="10"/>
-      <c r="R15" s="10"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="K16" t="s">
-        <v>66</v>
-      </c>
+      <c r="Q15" s="10"/>
+      <c r="S15" s="10"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="L16" t="s">
         <v>66</v>
       </c>
       <c r="M16" t="s">
+        <v>66</v>
+      </c>
+      <c r="N16" t="s">
         <v>58</v>
       </c>
-      <c r="N16">
+      <c r="O16">
         <v>2012</v>
       </c>
-      <c r="P16">
+      <c r="Q16">
         <v>2050</v>
       </c>
     </row>
-    <row r="17" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J17" s="1" t="s">
+    <row r="17" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K17" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
       <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
         <v>9999</v>
       </c>
-      <c r="M17" s="5">
+      <c r="N17" s="5">
         <v>68226787</v>
       </c>
-      <c r="N17" s="6">
+      <c r="O17" s="6">
         <v>0.01</v>
       </c>
-      <c r="O17">
-        <f>+M17*N17</f>
+      <c r="P17">
+        <f t="shared" ref="P17:P22" si="3">+N17*O17</f>
         <v>682267.87</v>
       </c>
-      <c r="P17" s="6">
+      <c r="Q17" s="6">
         <v>0.01</v>
       </c>
-      <c r="Q17">
-        <f>+M17*P17</f>
+      <c r="R17">
+        <f t="shared" ref="R17:R22" si="4">+N17*Q17</f>
         <v>682267.87</v>
       </c>
     </row>
-    <row r="18" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="K18">
+    <row r="18" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="L18">
         <v>10000</v>
       </c>
-      <c r="L18">
+      <c r="M18">
         <v>34999</v>
       </c>
-      <c r="M18" s="5">
+      <c r="N18" s="5">
         <v>1268561872</v>
       </c>
-      <c r="N18" s="6">
+      <c r="O18" s="6">
         <v>0.09</v>
       </c>
-      <c r="O18">
-        <f>+M18*N18</f>
+      <c r="P18">
+        <f t="shared" si="3"/>
         <v>114170568.47999999</v>
       </c>
-      <c r="P18" s="6">
+      <c r="Q18" s="6">
         <v>0.06</v>
       </c>
-      <c r="Q18">
-        <f>+M18*P18</f>
+      <c r="R18">
+        <f t="shared" si="4"/>
         <v>76113712.319999993</v>
       </c>
     </row>
-    <row r="19" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="K19">
+    <row r="19" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="L19">
         <v>35000</v>
       </c>
-      <c r="L19">
+      <c r="M19">
         <v>59999</v>
       </c>
-      <c r="M19" s="5">
+      <c r="N19" s="5">
         <v>2243075236</v>
       </c>
-      <c r="N19" s="6">
+      <c r="O19" s="6">
         <v>0.22</v>
       </c>
-      <c r="O19">
-        <f>+M19*N19</f>
+      <c r="P19">
+        <f t="shared" si="3"/>
         <v>493476551.92000002</v>
       </c>
-      <c r="P19" s="6">
+      <c r="Q19" s="6">
         <v>0.2</v>
       </c>
-      <c r="Q19">
-        <f>+M19*P19</f>
+      <c r="R19">
+        <f t="shared" si="4"/>
         <v>448615047.20000005</v>
       </c>
     </row>
-    <row r="20" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="K20">
+    <row r="20" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="L20">
         <v>60000</v>
       </c>
-      <c r="L20">
+      <c r="M20">
         <v>99999</v>
       </c>
-      <c r="M20" s="5">
+      <c r="N20" s="5">
         <v>3821361703</v>
       </c>
-      <c r="N20" s="6">
+      <c r="O20" s="6">
         <v>0.26</v>
       </c>
-      <c r="O20">
-        <f>+M20*N20</f>
+      <c r="P20">
+        <f t="shared" si="3"/>
         <v>993554042.78000009</v>
       </c>
-      <c r="P20" s="6">
+      <c r="Q20" s="6">
         <v>0.23</v>
       </c>
-      <c r="Q20">
-        <f>+M20*P20</f>
+      <c r="R20">
+        <f t="shared" si="4"/>
         <v>878913191.69000006</v>
       </c>
     </row>
-    <row r="21" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="K21">
+    <row r="21" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="L21">
         <v>100000</v>
       </c>
-      <c r="L21">
+      <c r="M21">
         <v>199999</v>
       </c>
-      <c r="M21" s="5">
+      <c r="N21" s="5">
         <v>7763260284</v>
       </c>
-      <c r="N21" s="6">
+      <c r="O21" s="6">
         <v>0.31</v>
       </c>
-      <c r="O21">
-        <f>+M21*N21</f>
+      <c r="P21">
+        <f t="shared" si="3"/>
         <v>2406610688.04</v>
       </c>
-      <c r="P21" s="6">
+      <c r="Q21" s="6">
         <v>0.4</v>
       </c>
-      <c r="Q21">
-        <f>+M21*P21</f>
+      <c r="R21">
+        <f t="shared" si="4"/>
         <v>3105304113.6000004</v>
       </c>
     </row>
-    <row r="22" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="K22">
+    <row r="22" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="L22">
         <v>200000</v>
       </c>
-      <c r="L22">
+      <c r="M22">
         <v>400000</v>
       </c>
-      <c r="M22" s="5">
+      <c r="N22" s="5">
         <v>10901043017</v>
       </c>
-      <c r="N22" s="6">
+      <c r="O22" s="6">
         <v>0.11</v>
       </c>
-      <c r="O22">
-        <f>+M22*N22</f>
+      <c r="P22">
+        <f t="shared" si="3"/>
         <v>1199114731.8700001</v>
       </c>
-      <c r="P22" s="6">
+      <c r="Q22" s="6">
         <v>0.1</v>
       </c>
-      <c r="Q22">
-        <f>+M22*P22</f>
+      <c r="R22">
+        <f t="shared" si="4"/>
         <v>1090104301.7</v>
       </c>
     </row>
-    <row r="23" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J23" t="s">
+    <row r="23" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K23" t="s">
         <v>69</v>
       </c>
-      <c r="N23" s="10">
-        <f>+AVERAGE(K17:L17)*N17+AVERAGE(K18:L18)*N18+AVERAGE(K19:L19)*N19+AVERAGE(K20:L20)*N20+AVERAGE(K21:L21)*N21+AVERAGE(K22:L22)*N22</f>
+      <c r="O23" s="10">
+        <f>+AVERAGE(L17:M17)*O17+AVERAGE(L18:M18)*O18+AVERAGE(L19:M19)*O19+AVERAGE(L20:M20)*O20+AVERAGE(L21:M21)*O21+AVERAGE(L22:M22)*O22</f>
         <v>112824.55499999999</v>
       </c>
-      <c r="P23" s="10">
-        <f>+AVERAGE(K17:L17)*P17+AVERAGE(K18:L18)*P18+AVERAGE(K19:L19)*P19+AVERAGE(K20:L20)*P20+AVERAGE(K21:L21)*P21+AVERAGE(K22:L22)*P22</f>
+      <c r="Q23" s="10">
+        <f>+AVERAGE(L17:M17)*Q17+AVERAGE(L18:M18)*Q18+AVERAGE(L19:M19)*Q19+AVERAGE(L20:M20)*Q20+AVERAGE(L21:M21)*Q21+AVERAGE(L22:M22)*Q22</f>
         <v>119299.55</v>
       </c>
-      <c r="R23" s="10">
-        <f>+AVERAGE(N23:P23)</f>
+      <c r="S23" s="10">
+        <f>+AVERAGE(O23:Q23)</f>
         <v>116062.05249999999</v>
       </c>
     </row>
-    <row r="24" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="N24" s="10"/>
-      <c r="P24" s="10"/>
-      <c r="R24" s="10"/>
-    </row>
-    <row r="25" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="K25" t="s">
-        <v>66</v>
-      </c>
+    <row r="24" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="O24" s="10"/>
+      <c r="Q24" s="10"/>
+      <c r="S24" s="10"/>
+    </row>
+    <row r="25" spans="11:19" x14ac:dyDescent="0.25">
       <c r="L25" t="s">
         <v>66</v>
       </c>
       <c r="M25" t="s">
+        <v>66</v>
+      </c>
+      <c r="N25" t="s">
         <v>58</v>
       </c>
-      <c r="N25">
+      <c r="O25">
         <v>2012</v>
       </c>
-      <c r="P25">
+      <c r="Q25">
         <v>2050</v>
       </c>
     </row>
-    <row r="26" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J26" s="1" t="s">
+    <row r="26" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K26" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K26">
-        <v>0</v>
-      </c>
       <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
         <v>4999</v>
       </c>
-      <c r="N26" s="6">
+      <c r="N26">
+        <v>91086398</v>
+      </c>
+      <c r="O26" s="6">
         <v>0.01</v>
       </c>
-      <c r="P26" s="6">
+      <c r="P26">
+        <f>+N26*O26</f>
+        <v>910863.98</v>
+      </c>
+      <c r="Q26" s="6">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="27" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="K27">
+      <c r="R26">
+        <f>+N26*Q26</f>
+        <v>910863.98</v>
+      </c>
+    </row>
+    <row r="27" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="L27">
         <v>5000</v>
       </c>
-      <c r="L27">
+      <c r="M27">
         <v>9999</v>
       </c>
-      <c r="N27" s="6">
+      <c r="N27">
+        <v>91086398</v>
+      </c>
+      <c r="O27" s="6">
         <v>0.01</v>
       </c>
-      <c r="P27" s="6">
+      <c r="P27">
+        <f t="shared" ref="P27:P33" si="5">+N27*O27</f>
+        <v>910863.98</v>
+      </c>
+      <c r="Q27" s="6">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="28" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="K28">
+      <c r="R27">
+        <f t="shared" ref="R27:R33" si="6">+N27*Q27</f>
+        <v>910863.98</v>
+      </c>
+    </row>
+    <row r="28" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="L28">
         <v>10000</v>
       </c>
-      <c r="L28">
+      <c r="M28">
         <v>19999</v>
       </c>
-      <c r="N28" s="6">
+      <c r="N28">
+        <v>1519025926</v>
+      </c>
+      <c r="O28" s="6">
         <v>0.01</v>
       </c>
-      <c r="P28" s="6">
+      <c r="P28">
+        <f t="shared" si="5"/>
+        <v>15190259.26</v>
+      </c>
+      <c r="Q28" s="6">
         <v>0.01</v>
       </c>
-    </row>
-    <row r="29" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="K29">
+      <c r="R28">
+        <f t="shared" si="6"/>
+        <v>15190259.26</v>
+      </c>
+    </row>
+    <row r="29" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="L29">
         <v>20000</v>
       </c>
-      <c r="L29">
+      <c r="M29">
         <v>59999</v>
       </c>
-      <c r="N29" s="6">
+      <c r="N29">
+        <v>1519025926</v>
+      </c>
+      <c r="O29" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="P29" s="6">
+      <c r="P29">
+        <f t="shared" si="5"/>
+        <v>106331814.82000001</v>
+      </c>
+      <c r="Q29" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="30" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="K30">
+      <c r="R29">
+        <f t="shared" si="6"/>
+        <v>106331814.82000001</v>
+      </c>
+    </row>
+    <row r="30" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="L30">
         <v>60000</v>
       </c>
-      <c r="L30">
+      <c r="M30">
         <v>79999</v>
       </c>
-      <c r="N30" s="6">
+      <c r="N30">
+        <v>2629911081</v>
+      </c>
+      <c r="O30" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="P30" s="6">
+      <c r="P30">
+        <f t="shared" si="5"/>
+        <v>184093775.67000002</v>
+      </c>
+      <c r="Q30" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="31" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="K31">
+      <c r="R30">
+        <f t="shared" si="6"/>
+        <v>184093775.67000002</v>
+      </c>
+    </row>
+    <row r="31" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="L31">
         <v>80000</v>
       </c>
-      <c r="L31">
+      <c r="M31">
         <v>119999</v>
       </c>
-      <c r="N31" s="6">
+      <c r="N31">
+        <v>4417734613</v>
+      </c>
+      <c r="O31" s="6">
         <v>0.23</v>
       </c>
-      <c r="P31" s="6">
+      <c r="P31">
+        <f t="shared" si="5"/>
+        <v>1016078960.99</v>
+      </c>
+      <c r="Q31" s="6">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="32" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="K32">
+      <c r="R31">
+        <f t="shared" si="6"/>
+        <v>1016078960.99</v>
+      </c>
+    </row>
+    <row r="32" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="L32">
         <v>120000</v>
       </c>
-      <c r="L32">
+      <c r="M32">
         <v>199999</v>
       </c>
-      <c r="N32" s="6">
+      <c r="N32">
+        <v>7024437504</v>
+      </c>
+      <c r="O32" s="6">
         <v>0.17</v>
       </c>
-      <c r="P32" s="6">
+      <c r="P32">
+        <f t="shared" si="5"/>
+        <v>1194154375.6800001</v>
+      </c>
+      <c r="Q32" s="6">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="33" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="K33">
-        <v>200000</v>
-      </c>
+      <c r="R32">
+        <f t="shared" si="6"/>
+        <v>1194154375.6800001</v>
+      </c>
+    </row>
+    <row r="33" spans="11:19" x14ac:dyDescent="0.25">
       <c r="L33">
         <v>200000</v>
       </c>
-      <c r="N33" s="6">
+      <c r="M33">
+        <v>200000</v>
+      </c>
+      <c r="N33">
+        <v>14197046742</v>
+      </c>
+      <c r="O33" s="6">
         <v>0.43</v>
       </c>
-      <c r="P33" s="6">
+      <c r="P33">
+        <f t="shared" si="5"/>
+        <v>6104730099.0599995</v>
+      </c>
+      <c r="Q33" s="6">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="34" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J34" t="s">
+      <c r="R33">
+        <f t="shared" si="6"/>
+        <v>6104730099.0599995</v>
+      </c>
+    </row>
+    <row r="34" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K34" t="s">
         <v>69</v>
       </c>
-      <c r="N34" s="10">
-        <f>+AVERAGE(K26:L26)*N26+AVERAGE(K27:L27)*N27+AVERAGE(K28:L28)*N28+AVERAGE(K29:L29)*N29+AVERAGE(K30:L30)*N30+AVERAGE(K31:L31)*N31+AVERAGE(K32:L32)*N32+AVERAGE(K33:L33)*N33</f>
+      <c r="O34" s="10">
+        <f>+AVERAGE(L26:M26)*O26+AVERAGE(L27:M27)*O27+AVERAGE(L28:M28)*O28+AVERAGE(L29:M29)*O29+AVERAGE(L30:M30)*O30+AVERAGE(L31:M31)*O31+AVERAGE(L32:M32)*O32+AVERAGE(L33:M33)*O33</f>
         <v>144149.715</v>
       </c>
-      <c r="P34" s="10">
-        <f>+AVERAGE(K26:L26)*P26+AVERAGE(K27:L27)*P27+AVERAGE(K28:L28)*P28+AVERAGE(K29:L29)*P29+AVERAGE(K30:L30)*P30+AVERAGE(K31:L31)*P31+AVERAGE(K32:L32)*P32+AVERAGE(K33:L33)*P33</f>
+      <c r="Q34" s="10">
+        <f>+AVERAGE(L26:M26)*Q26+AVERAGE(L27:M27)*Q27+AVERAGE(L28:M28)*Q28+AVERAGE(L29:M29)*Q29+AVERAGE(L30:M30)*Q30+AVERAGE(L31:M31)*Q31+AVERAGE(L32:M32)*Q32+AVERAGE(L33:M33)*Q33</f>
         <v>144149.715</v>
       </c>
-      <c r="R34" s="10">
-        <f>+AVERAGE(N34:P34)</f>
+      <c r="S34" s="10">
+        <f>+AVERAGE(O34:Q34)</f>
         <v>144149.715</v>
       </c>
     </row>
-    <row r="35" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="N35" s="10"/>
-      <c r="P35" s="10"/>
-      <c r="R35" s="10"/>
-    </row>
-    <row r="36" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="K36" t="s">
-        <v>66</v>
-      </c>
+    <row r="35" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="O35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="S35" s="10"/>
+    </row>
+    <row r="36" spans="11:19" x14ac:dyDescent="0.25">
       <c r="L36" t="s">
         <v>66</v>
       </c>
       <c r="M36" t="s">
+        <v>66</v>
+      </c>
+      <c r="N36" t="s">
         <v>58</v>
       </c>
-      <c r="N36" t="s">
+      <c r="O36" t="s">
         <v>68</v>
       </c>
-      <c r="O36" t="s">
+      <c r="P36" t="s">
         <v>69</v>
       </c>
-      <c r="P36" t="s">
+      <c r="Q36" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="37" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J37" s="1" t="s">
+    <row r="37" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K37" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="K37">
-        <v>0</v>
-      </c>
       <c r="L37">
+        <v>0</v>
+      </c>
+      <c r="M37">
         <v>4999</v>
       </c>
-      <c r="M37">
+      <c r="N37">
         <v>76945792</v>
       </c>
-      <c r="N37">
+      <c r="O37">
         <v>11620</v>
       </c>
-      <c r="O37">
+      <c r="P37">
         <v>1925</v>
       </c>
-      <c r="P37">
+      <c r="Q37">
         <v>1119</v>
       </c>
     </row>
-    <row r="38" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="K38">
+    <row r="38" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="L38">
         <v>5000</v>
       </c>
-      <c r="L38">
+      <c r="M38">
         <v>9999</v>
       </c>
-      <c r="M38">
+      <c r="N38">
         <v>365344150</v>
       </c>
-      <c r="N38">
+      <c r="O38">
         <v>2894</v>
       </c>
-      <c r="O38">
+      <c r="P38">
         <v>7339</v>
       </c>
-      <c r="P38">
+      <c r="Q38">
         <v>3320</v>
       </c>
     </row>
-    <row r="39" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="K39">
+    <row r="39" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="L39">
         <v>10000</v>
       </c>
-      <c r="M39">
+      <c r="N39">
         <v>866510887</v>
       </c>
-      <c r="N39">
+      <c r="O39">
         <v>1972</v>
       </c>
-      <c r="O39">
+      <c r="P39">
         <v>22472</v>
       </c>
-      <c r="P39">
+      <c r="Q39">
         <v>7418</v>
       </c>
     </row>
-    <row r="40" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J40" t="s">
+    <row r="40" spans="11:19" x14ac:dyDescent="0.25">
+      <c r="K40" t="s">
         <v>72</v>
       </c>
-      <c r="O40" s="10">
-        <f>+(N37/SUM(N37:N39))*O37+(N38/SUM(N37:N39))*O38+(N39/SUM(N37:N39))*O39</f>
+      <c r="P40" s="10">
+        <f>+(O37/SUM(O37:O39))*P37+(O38/SUM(O37:O39))*P38+(O39/SUM(O37:O39))*P39</f>
         <v>5333.1523717093296</v>
       </c>
-      <c r="P40" s="10">
-        <f>+(N37/SUM(N37:N39))*P37+(N38/SUM(N37:N39))*P38+(N39/SUM(N37:N39))*P39</f>
+      <c r="Q40" s="10">
+        <f>+(O37/SUM(O37:O39))*Q37+(O38/SUM(O37:O39))*Q38+(O39/SUM(O37:O39))*Q39</f>
         <v>2258.8351328399854</v>
       </c>
     </row>
-    <row r="50" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B50" s="2"/>
+    <row r="50" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
@@ -1744,9 +1856,9 @@
       <c r="AI50" s="2"/>
       <c r="AJ50" s="2"/>
       <c r="AK50" s="2"/>
-    </row>
-    <row r="51" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B51" s="4"/>
+      <c r="AL50" s="2"/>
+    </row>
+    <row r="51" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C51" s="4"/>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
@@ -1782,9 +1894,9 @@
       <c r="AI51" s="4"/>
       <c r="AJ51" s="4"/>
       <c r="AK51" s="4"/>
-    </row>
-    <row r="52" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B52" s="4"/>
+      <c r="AL51" s="4"/>
+    </row>
+    <row r="52" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
@@ -1820,9 +1932,9 @@
       <c r="AI52" s="4"/>
       <c r="AJ52" s="4"/>
       <c r="AK52" s="4"/>
-    </row>
-    <row r="53" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B53" s="4"/>
+      <c r="AL52" s="4"/>
+    </row>
+    <row r="53" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
@@ -1858,9 +1970,9 @@
       <c r="AI53" s="4"/>
       <c r="AJ53" s="4"/>
       <c r="AK53" s="4"/>
-    </row>
-    <row r="54" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B54" s="4"/>
+      <c r="AL53" s="4"/>
+    </row>
+    <row r="54" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
@@ -1896,9 +2008,9 @@
       <c r="AI54" s="4"/>
       <c r="AJ54" s="4"/>
       <c r="AK54" s="4"/>
-    </row>
-    <row r="55" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B55" s="4"/>
+      <c r="AL54" s="4"/>
+    </row>
+    <row r="55" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
       <c r="E55" s="4"/>
@@ -1934,9 +2046,9 @@
       <c r="AI55" s="4"/>
       <c r="AJ55" s="4"/>
       <c r="AK55" s="4"/>
-    </row>
-    <row r="56" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B56" s="4"/>
+      <c r="AL55" s="4"/>
+    </row>
+    <row r="56" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
       <c r="E56" s="4"/>
@@ -1972,9 +2084,9 @@
       <c r="AI56" s="4"/>
       <c r="AJ56" s="4"/>
       <c r="AK56" s="4"/>
-    </row>
-    <row r="57" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B57" s="4"/>
+      <c r="AL56" s="4"/>
+    </row>
+    <row r="57" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
       <c r="E57" s="4"/>
@@ -2010,9 +2122,9 @@
       <c r="AI57" s="4"/>
       <c r="AJ57" s="4"/>
       <c r="AK57" s="4"/>
-    </row>
-    <row r="58" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B58" s="4"/>
+      <c r="AL57" s="4"/>
+    </row>
+    <row r="58" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
       <c r="E58" s="4"/>
@@ -2048,9 +2160,9 @@
       <c r="AI58" s="4"/>
       <c r="AJ58" s="4"/>
       <c r="AK58" s="4"/>
-    </row>
-    <row r="59" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B59" s="4"/>
+      <c r="AL58" s="4"/>
+    </row>
+    <row r="59" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
       <c r="E59" s="4"/>
@@ -2086,9 +2198,9 @@
       <c r="AI59" s="4"/>
       <c r="AJ59" s="4"/>
       <c r="AK59" s="4"/>
-    </row>
-    <row r="60" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B60" s="4"/>
+      <c r="AL59" s="4"/>
+    </row>
+    <row r="60" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
@@ -2124,9 +2236,9 @@
       <c r="AI60" s="4"/>
       <c r="AJ60" s="4"/>
       <c r="AK60" s="4"/>
-    </row>
-    <row r="61" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B61" s="4"/>
+      <c r="AL60" s="4"/>
+    </row>
+    <row r="61" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
@@ -2162,9 +2274,9 @@
       <c r="AI61" s="4"/>
       <c r="AJ61" s="4"/>
       <c r="AK61" s="4"/>
-    </row>
-    <row r="62" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B62" s="4"/>
+      <c r="AL61" s="4"/>
+    </row>
+    <row r="62" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
@@ -2200,9 +2312,9 @@
       <c r="AI62" s="4"/>
       <c r="AJ62" s="4"/>
       <c r="AK62" s="4"/>
-    </row>
-    <row r="63" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B63" s="4"/>
+      <c r="AL62" s="4"/>
+    </row>
+    <row r="63" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
@@ -2238,9 +2350,9 @@
       <c r="AI63" s="4"/>
       <c r="AJ63" s="4"/>
       <c r="AK63" s="4"/>
-    </row>
-    <row r="64" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B64" s="4"/>
+      <c r="AL63" s="4"/>
+    </row>
+    <row r="64" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
@@ -2276,9 +2388,9 @@
       <c r="AI64" s="4"/>
       <c r="AJ64" s="4"/>
       <c r="AK64" s="4"/>
-    </row>
-    <row r="65" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B65" s="4"/>
+      <c r="AL64" s="4"/>
+    </row>
+    <row r="65" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C65" s="4"/>
       <c r="D65" s="4"/>
       <c r="E65" s="4"/>
@@ -2314,9 +2426,9 @@
       <c r="AI65" s="4"/>
       <c r="AJ65" s="4"/>
       <c r="AK65" s="4"/>
-    </row>
-    <row r="66" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B66" s="4"/>
+      <c r="AL65" s="4"/>
+    </row>
+    <row r="66" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C66" s="4"/>
       <c r="D66" s="4"/>
       <c r="E66" s="4"/>
@@ -2352,9 +2464,9 @@
       <c r="AI66" s="4"/>
       <c r="AJ66" s="4"/>
       <c r="AK66" s="4"/>
-    </row>
-    <row r="67" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B67" s="4"/>
+      <c r="AL66" s="4"/>
+    </row>
+    <row r="67" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C67" s="4"/>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
@@ -2390,9 +2502,9 @@
       <c r="AI67" s="4"/>
       <c r="AJ67" s="4"/>
       <c r="AK67" s="4"/>
-    </row>
-    <row r="68" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B68" s="4"/>
+      <c r="AL67" s="4"/>
+    </row>
+    <row r="68" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
       <c r="E68" s="4"/>
@@ -2428,9 +2540,9 @@
       <c r="AI68" s="4"/>
       <c r="AJ68" s="4"/>
       <c r="AK68" s="4"/>
-    </row>
-    <row r="69" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B69" s="4"/>
+      <c r="AL68" s="4"/>
+    </row>
+    <row r="69" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
       <c r="E69" s="4"/>
@@ -2466,9 +2578,9 @@
       <c r="AI69" s="4"/>
       <c r="AJ69" s="4"/>
       <c r="AK69" s="4"/>
-    </row>
-    <row r="70" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B70" s="4"/>
+      <c r="AL69" s="4"/>
+    </row>
+    <row r="70" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
       <c r="E70" s="4"/>
@@ -2504,9 +2616,9 @@
       <c r="AI70" s="4"/>
       <c r="AJ70" s="4"/>
       <c r="AK70" s="4"/>
-    </row>
-    <row r="71" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B71" s="4"/>
+      <c r="AL70" s="4"/>
+    </row>
+    <row r="71" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
       <c r="E71" s="4"/>
@@ -2542,9 +2654,9 @@
       <c r="AI71" s="4"/>
       <c r="AJ71" s="4"/>
       <c r="AK71" s="4"/>
-    </row>
-    <row r="72" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B72" s="4"/>
+      <c r="AL71" s="4"/>
+    </row>
+    <row r="72" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C72" s="4"/>
       <c r="D72" s="4"/>
       <c r="E72" s="4"/>
@@ -2580,9 +2692,9 @@
       <c r="AI72" s="4"/>
       <c r="AJ72" s="4"/>
       <c r="AK72" s="4"/>
-    </row>
-    <row r="73" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B73" s="4"/>
+      <c r="AL72" s="4"/>
+    </row>
+    <row r="73" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C73" s="4"/>
       <c r="D73" s="4"/>
       <c r="E73" s="4"/>
@@ -2618,9 +2730,9 @@
       <c r="AI73" s="4"/>
       <c r="AJ73" s="4"/>
       <c r="AK73" s="4"/>
-    </row>
-    <row r="74" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B74" s="4"/>
+      <c r="AL73" s="4"/>
+    </row>
+    <row r="74" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C74" s="4"/>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
@@ -2656,9 +2768,9 @@
       <c r="AI74" s="4"/>
       <c r="AJ74" s="4"/>
       <c r="AK74" s="4"/>
-    </row>
-    <row r="75" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B75" s="4"/>
+      <c r="AL74" s="4"/>
+    </row>
+    <row r="75" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C75" s="4"/>
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
@@ -2694,9 +2806,9 @@
       <c r="AI75" s="4"/>
       <c r="AJ75" s="4"/>
       <c r="AK75" s="4"/>
-    </row>
-    <row r="76" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B76" s="4"/>
+      <c r="AL75" s="4"/>
+    </row>
+    <row r="76" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C76" s="4"/>
       <c r="D76" s="4"/>
       <c r="E76" s="4"/>
@@ -2732,9 +2844,9 @@
       <c r="AI76" s="4"/>
       <c r="AJ76" s="4"/>
       <c r="AK76" s="4"/>
-    </row>
-    <row r="77" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B77" s="4"/>
+      <c r="AL76" s="4"/>
+    </row>
+    <row r="77" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C77" s="4"/>
       <c r="D77" s="4"/>
       <c r="E77" s="4"/>
@@ -2770,9 +2882,9 @@
       <c r="AI77" s="4"/>
       <c r="AJ77" s="4"/>
       <c r="AK77" s="4"/>
-    </row>
-    <row r="78" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B78" s="4"/>
+      <c r="AL77" s="4"/>
+    </row>
+    <row r="78" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
       <c r="E78" s="4"/>
@@ -2808,9 +2920,9 @@
       <c r="AI78" s="4"/>
       <c r="AJ78" s="4"/>
       <c r="AK78" s="4"/>
-    </row>
-    <row r="79" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B79" s="4"/>
+      <c r="AL78" s="4"/>
+    </row>
+    <row r="79" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
       <c r="E79" s="4"/>
@@ -2846,9 +2958,9 @@
       <c r="AI79" s="4"/>
       <c r="AJ79" s="4"/>
       <c r="AK79" s="4"/>
-    </row>
-    <row r="80" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B80" s="4"/>
+      <c r="AL79" s="4"/>
+    </row>
+    <row r="80" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
       <c r="E80" s="4"/>
@@ -2884,9 +2996,9 @@
       <c r="AI80" s="4"/>
       <c r="AJ80" s="4"/>
       <c r="AK80" s="4"/>
-    </row>
-    <row r="81" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B81" s="4"/>
+      <c r="AL80" s="4"/>
+    </row>
+    <row r="81" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
       <c r="E81" s="4"/>
@@ -2922,9 +3034,9 @@
       <c r="AI81" s="4"/>
       <c r="AJ81" s="4"/>
       <c r="AK81" s="4"/>
-    </row>
-    <row r="82" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B82" s="4"/>
+      <c r="AL81" s="4"/>
+    </row>
+    <row r="82" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
       <c r="E82" s="4"/>
@@ -2960,9 +3072,9 @@
       <c r="AI82" s="4"/>
       <c r="AJ82" s="4"/>
       <c r="AK82" s="4"/>
-    </row>
-    <row r="83" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B83" s="4"/>
+      <c r="AL82" s="4"/>
+    </row>
+    <row r="83" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
       <c r="E83" s="4"/>
@@ -2998,9 +3110,9 @@
       <c r="AI83" s="4"/>
       <c r="AJ83" s="4"/>
       <c r="AK83" s="4"/>
-    </row>
-    <row r="84" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B84" s="4"/>
+      <c r="AL83" s="4"/>
+    </row>
+    <row r="84" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
       <c r="E84" s="4"/>
@@ -3036,9 +3148,9 @@
       <c r="AI84" s="4"/>
       <c r="AJ84" s="4"/>
       <c r="AK84" s="4"/>
-    </row>
-    <row r="85" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B85" s="4"/>
+      <c r="AL84" s="4"/>
+    </row>
+    <row r="85" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
       <c r="E85" s="4"/>
@@ -3074,9 +3186,9 @@
       <c r="AI85" s="4"/>
       <c r="AJ85" s="4"/>
       <c r="AK85" s="4"/>
-    </row>
-    <row r="86" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B86" s="4"/>
+      <c r="AL85" s="4"/>
+    </row>
+    <row r="86" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C86" s="4"/>
       <c r="D86" s="4"/>
       <c r="E86" s="4"/>
@@ -3112,9 +3224,9 @@
       <c r="AI86" s="4"/>
       <c r="AJ86" s="4"/>
       <c r="AK86" s="4"/>
-    </row>
-    <row r="87" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B87" s="4"/>
+      <c r="AL86" s="4"/>
+    </row>
+    <row r="87" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C87" s="4"/>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
@@ -3150,9 +3262,9 @@
       <c r="AI87" s="4"/>
       <c r="AJ87" s="4"/>
       <c r="AK87" s="4"/>
-    </row>
-    <row r="88" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B88" s="4"/>
+      <c r="AL87" s="4"/>
+    </row>
+    <row r="88" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
       <c r="E88" s="4"/>
@@ -3188,9 +3300,9 @@
       <c r="AI88" s="4"/>
       <c r="AJ88" s="4"/>
       <c r="AK88" s="4"/>
-    </row>
-    <row r="89" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B89" s="4"/>
+      <c r="AL88" s="4"/>
+    </row>
+    <row r="89" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
@@ -3226,9 +3338,9 @@
       <c r="AI89" s="4"/>
       <c r="AJ89" s="4"/>
       <c r="AK89" s="4"/>
-    </row>
-    <row r="90" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B90" s="4"/>
+      <c r="AL89" s="4"/>
+    </row>
+    <row r="90" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
       <c r="E90" s="4"/>
@@ -3264,9 +3376,9 @@
       <c r="AI90" s="4"/>
       <c r="AJ90" s="4"/>
       <c r="AK90" s="4"/>
-    </row>
-    <row r="91" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B91" s="4"/>
+      <c r="AL90" s="4"/>
+    </row>
+    <row r="91" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
       <c r="E91" s="4"/>
@@ -3302,9 +3414,9 @@
       <c r="AI91" s="4"/>
       <c r="AJ91" s="4"/>
       <c r="AK91" s="4"/>
-    </row>
-    <row r="92" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B92" s="4"/>
+      <c r="AL91" s="4"/>
+    </row>
+    <row r="92" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
       <c r="E92" s="4"/>
@@ -3340,9 +3452,9 @@
       <c r="AI92" s="4"/>
       <c r="AJ92" s="4"/>
       <c r="AK92" s="4"/>
-    </row>
-    <row r="93" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B93" s="4"/>
+      <c r="AL92" s="4"/>
+    </row>
+    <row r="93" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
       <c r="E93" s="4"/>
@@ -3378,9 +3490,9 @@
       <c r="AI93" s="4"/>
       <c r="AJ93" s="4"/>
       <c r="AK93" s="4"/>
-    </row>
-    <row r="94" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B94" s="4"/>
+      <c r="AL93" s="4"/>
+    </row>
+    <row r="94" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
       <c r="E94" s="4"/>
@@ -3416,9 +3528,9 @@
       <c r="AI94" s="4"/>
       <c r="AJ94" s="4"/>
       <c r="AK94" s="4"/>
-    </row>
-    <row r="95" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B95" s="4"/>
+      <c r="AL94" s="4"/>
+    </row>
+    <row r="95" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
       <c r="E95" s="4"/>
@@ -3454,9 +3566,9 @@
       <c r="AI95" s="4"/>
       <c r="AJ95" s="4"/>
       <c r="AK95" s="4"/>
-    </row>
-    <row r="96" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B96" s="4"/>
+      <c r="AL95" s="4"/>
+    </row>
+    <row r="96" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
       <c r="E96" s="4"/>
@@ -3492,9 +3604,9 @@
       <c r="AI96" s="4"/>
       <c r="AJ96" s="4"/>
       <c r="AK96" s="4"/>
-    </row>
-    <row r="97" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B97" s="4"/>
+      <c r="AL96" s="4"/>
+    </row>
+    <row r="97" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
       <c r="E97" s="4"/>
@@ -3530,9 +3642,9 @@
       <c r="AI97" s="4"/>
       <c r="AJ97" s="4"/>
       <c r="AK97" s="4"/>
-    </row>
-    <row r="98" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B98" s="4"/>
+      <c r="AL97" s="4"/>
+    </row>
+    <row r="98" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
       <c r="E98" s="4"/>
@@ -3568,9 +3680,9 @@
       <c r="AI98" s="4"/>
       <c r="AJ98" s="4"/>
       <c r="AK98" s="4"/>
-    </row>
-    <row r="99" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B99" s="4"/>
+      <c r="AL98" s="4"/>
+    </row>
+    <row r="99" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
       <c r="E99" s="4"/>
@@ -3606,9 +3718,9 @@
       <c r="AI99" s="4"/>
       <c r="AJ99" s="4"/>
       <c r="AK99" s="4"/>
-    </row>
-    <row r="100" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B100" s="4"/>
+      <c r="AL99" s="4"/>
+    </row>
+    <row r="100" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
       <c r="E100" s="4"/>
@@ -3644,9 +3756,9 @@
       <c r="AI100" s="4"/>
       <c r="AJ100" s="4"/>
       <c r="AK100" s="4"/>
-    </row>
-    <row r="101" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B101" s="4"/>
+      <c r="AL100" s="4"/>
+    </row>
+    <row r="101" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C101" s="4"/>
       <c r="D101" s="4"/>
       <c r="E101" s="4"/>
@@ -3682,9 +3794,9 @@
       <c r="AI101" s="4"/>
       <c r="AJ101" s="4"/>
       <c r="AK101" s="4"/>
-    </row>
-    <row r="102" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B102" s="4"/>
+      <c r="AL101" s="4"/>
+    </row>
+    <row r="102" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
       <c r="E102" s="4"/>
@@ -3720,9 +3832,9 @@
       <c r="AI102" s="4"/>
       <c r="AJ102" s="4"/>
       <c r="AK102" s="4"/>
-    </row>
-    <row r="103" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B103" s="4"/>
+      <c r="AL102" s="4"/>
+    </row>
+    <row r="103" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
       <c r="E103" s="4"/>
@@ -3758,9 +3870,9 @@
       <c r="AI103" s="4"/>
       <c r="AJ103" s="4"/>
       <c r="AK103" s="4"/>
-    </row>
-    <row r="104" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B104" s="4"/>
+      <c r="AL103" s="4"/>
+    </row>
+    <row r="104" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
       <c r="E104" s="4"/>
@@ -3796,9 +3908,9 @@
       <c r="AI104" s="4"/>
       <c r="AJ104" s="4"/>
       <c r="AK104" s="4"/>
-    </row>
-    <row r="105" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B105" s="4"/>
+      <c r="AL104" s="4"/>
+    </row>
+    <row r="105" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
       <c r="E105" s="4"/>
@@ -3834,9 +3946,9 @@
       <c r="AI105" s="4"/>
       <c r="AJ105" s="4"/>
       <c r="AK105" s="4"/>
-    </row>
-    <row r="106" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B106" s="4"/>
+      <c r="AL105" s="4"/>
+    </row>
+    <row r="106" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
       <c r="E106" s="4"/>
@@ -3872,9 +3984,9 @@
       <c r="AI106" s="4"/>
       <c r="AJ106" s="4"/>
       <c r="AK106" s="4"/>
-    </row>
-    <row r="107" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B107" s="4"/>
+      <c r="AL106" s="4"/>
+    </row>
+    <row r="107" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C107" s="4"/>
       <c r="D107" s="4"/>
       <c r="E107" s="4"/>
@@ -3910,9 +4022,9 @@
       <c r="AI107" s="4"/>
       <c r="AJ107" s="4"/>
       <c r="AK107" s="4"/>
-    </row>
-    <row r="108" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B108" s="4"/>
+      <c r="AL107" s="4"/>
+    </row>
+    <row r="108" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
       <c r="E108" s="4"/>
@@ -3948,9 +4060,9 @@
       <c r="AI108" s="4"/>
       <c r="AJ108" s="4"/>
       <c r="AK108" s="4"/>
-    </row>
-    <row r="109" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B109" s="4"/>
+      <c r="AL108" s="4"/>
+    </row>
+    <row r="109" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
       <c r="E109" s="4"/>
@@ -3986,9 +4098,9 @@
       <c r="AI109" s="4"/>
       <c r="AJ109" s="4"/>
       <c r="AK109" s="4"/>
-    </row>
-    <row r="110" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B110" s="4"/>
+      <c r="AL109" s="4"/>
+    </row>
+    <row r="110" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C110" s="4"/>
       <c r="D110" s="4"/>
       <c r="E110" s="4"/>
@@ -4024,9 +4136,9 @@
       <c r="AI110" s="4"/>
       <c r="AJ110" s="4"/>
       <c r="AK110" s="4"/>
-    </row>
-    <row r="111" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B111" s="4"/>
+      <c r="AL110" s="4"/>
+    </row>
+    <row r="111" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C111" s="4"/>
       <c r="D111" s="4"/>
       <c r="E111" s="4"/>
@@ -4062,9 +4174,9 @@
       <c r="AI111" s="4"/>
       <c r="AJ111" s="4"/>
       <c r="AK111" s="4"/>
-    </row>
-    <row r="112" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B112" s="4"/>
+      <c r="AL111" s="4"/>
+    </row>
+    <row r="112" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
       <c r="E112" s="4"/>
@@ -4100,9 +4212,9 @@
       <c r="AI112" s="4"/>
       <c r="AJ112" s="4"/>
       <c r="AK112" s="4"/>
-    </row>
-    <row r="113" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B113" s="4"/>
+      <c r="AL112" s="4"/>
+    </row>
+    <row r="113" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
       <c r="E113" s="4"/>
@@ -4138,9 +4250,9 @@
       <c r="AI113" s="4"/>
       <c r="AJ113" s="4"/>
       <c r="AK113" s="4"/>
-    </row>
-    <row r="114" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B114" s="4"/>
+      <c r="AL113" s="4"/>
+    </row>
+    <row r="114" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C114" s="4"/>
       <c r="D114" s="4"/>
       <c r="E114" s="4"/>
@@ -4176,9 +4288,9 @@
       <c r="AI114" s="4"/>
       <c r="AJ114" s="4"/>
       <c r="AK114" s="4"/>
-    </row>
-    <row r="115" spans="2:37" x14ac:dyDescent="0.25">
-      <c r="B115" s="4"/>
+      <c r="AL114" s="4"/>
+    </row>
+    <row r="115" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C115" s="4"/>
       <c r="D115" s="4"/>
       <c r="E115" s="4"/>
@@ -4214,6 +4326,7 @@
       <c r="AI115" s="4"/>
       <c r="AJ115" s="4"/>
       <c r="AK115" s="4"/>
+      <c r="AL115" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>